<commit_message>
feat: Sistema adaptado al flujo completo del Trello Las-Lira
CAMBIOS PRINCIPALES:
- Estados actualizados: Pedido → Pedidos Semana → Entregas para Mañana → Entregas de Hoy → En Proceso → Listo para Despacho → Despachados
- Sistema de etiquetas implementado:
  * Días de la semana (LUNES-DOMINGO) con colores
  * Estado de pago (Pagado/No Pagado/Falta Boleta o Factura)
  * Tipo de pedido (EVENTO/MANTENCIONES/Normal)
- Nuevo campo: cobranza (boleta/factura)
- Nuevo campo: foto_enviado_url (trazabilidad)
- Tarjetas muestran: nombre + teléfono + etiquetas + foto
- Flexibilidad de pago implementada
- Excel actualizado con todos los nuevos campos
</commit_message>
<xml_diff>
--- a/04_Pedidos.xlsx
+++ b/04_Pedidos.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q10"/>
+  <dimension ref="A1:V10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -438,20 +438,25 @@
     <col width="10" customWidth="1" min="1" max="1"/>
     <col width="16" customWidth="1" min="2" max="2"/>
     <col width="16" customWidth="1" min="3" max="3"/>
-    <col width="10" customWidth="1" min="4" max="4"/>
-    <col width="15" customWidth="1" min="5" max="5"/>
-    <col width="18" customWidth="1" min="6" max="6"/>
-    <col width="15" customWidth="1" min="7" max="7"/>
-    <col width="25" customWidth="1" min="8" max="8"/>
+    <col width="12" customWidth="1" min="4" max="4"/>
+    <col width="10" customWidth="1" min="5" max="5"/>
+    <col width="15" customWidth="1" min="6" max="6"/>
+    <col width="18" customWidth="1" min="7" max="7"/>
+    <col width="15" customWidth="1" min="8" max="8"/>
     <col width="25" customWidth="1" min="9" max="9"/>
-    <col width="12" customWidth="1" min="10" max="10"/>
+    <col width="25" customWidth="1" min="10" max="10"/>
     <col width="12" customWidth="1" min="11" max="11"/>
-    <col width="18" customWidth="1" min="12" max="12"/>
-    <col width="30" customWidth="1" min="13" max="13"/>
-    <col width="20" customWidth="1" min="14" max="14"/>
-    <col width="35" customWidth="1" min="15" max="15"/>
-    <col width="15" customWidth="1" min="16" max="16"/>
+    <col width="12" customWidth="1" min="12" max="12"/>
+    <col width="18" customWidth="1" min="13" max="13"/>
+    <col width="30" customWidth="1" min="14" max="14"/>
+    <col width="20" customWidth="1" min="15" max="15"/>
+    <col width="35" customWidth="1" min="16" max="16"/>
     <col width="15" customWidth="1" min="17" max="17"/>
+    <col width="18" customWidth="1" min="18" max="18"/>
+    <col width="15" customWidth="1" min="19" max="19"/>
+    <col width="15" customWidth="1" min="20" max="20"/>
+    <col width="25" customWidth="1" min="21" max="21"/>
+    <col width="25" customWidth="1" min="22" max="22"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -472,72 +477,97 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>Día Entrega</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
           <t>Canal</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Nro Pedido Shopify</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Nombre Cliente</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Celular</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Arreglo Pedido</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>Detalles Adicionales</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Precio Ramo</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>Precio Envío</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>Para (Destinatario)</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>Mensaje</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>Firma</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>Dirección</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>Motivo</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>Estado</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>Estado Pago</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>Tipo Pedido</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>Cobranza</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>Foto Enviado</t>
         </is>
       </c>
     </row>
@@ -559,70 +589,91 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
+          <t>LUNES</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
           <t>Shopify</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="F2" t="inlineStr">
         <is>
           <t>#SH1234</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="G2" t="inlineStr">
         <is>
           <t>María González</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="H2" t="inlineStr">
         <is>
           <t>+56912345601</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
+      <c r="I2" t="inlineStr">
         <is>
           <t>Pasión Roja</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr">
+      <c r="J2" t="inlineStr">
         <is>
           <t>Sin cambios</t>
         </is>
       </c>
-      <c r="J2" t="n">
+      <c r="K2" t="n">
         <v>35000</v>
       </c>
-      <c r="K2" t="n">
+      <c r="L2" t="n">
         <v>5000</v>
       </c>
-      <c r="L2" t="inlineStr">
+      <c r="M2" t="inlineStr">
         <is>
           <t>Ana González</t>
         </is>
       </c>
-      <c r="M2" t="inlineStr">
+      <c r="N2" t="inlineStr">
         <is>
           <t>Feliz cumpleaños hermana</t>
         </is>
       </c>
-      <c r="N2" t="inlineStr">
+      <c r="O2" t="inlineStr">
         <is>
           <t>Con cariño, María</t>
         </is>
       </c>
-      <c r="O2" t="inlineStr">
+      <c r="P2" t="inlineStr">
         <is>
           <t>Av. Las Condes 12345, Las Condes</t>
         </is>
       </c>
-      <c r="P2" t="inlineStr">
+      <c r="Q2" t="inlineStr">
         <is>
           <t>Cumpleaños</t>
         </is>
       </c>
-      <c r="Q2" t="inlineStr">
-        <is>
-          <t>Entregado</t>
-        </is>
-      </c>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>Despachados</t>
+        </is>
+      </c>
+      <c r="S2" t="inlineStr">
+        <is>
+          <t>Pagado</t>
+        </is>
+      </c>
+      <c r="T2" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="U2" t="inlineStr">
+        <is>
+          <t>BOLETA 11248 TR. 21/10/25</t>
+        </is>
+      </c>
+      <c r="V2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -642,64 +693,89 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
+          <t>MARTES</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
           <t>WhatsApp</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr">
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr">
         <is>
           <t>Carlos Pérez</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
+      <c r="H3" t="inlineStr">
         <is>
           <t>+56912345602</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr">
+      <c r="I3" t="inlineStr">
         <is>
           <t>Arreglo personalizado tonos rosados</t>
         </is>
       </c>
-      <c r="I3" t="inlineStr">
+      <c r="J3" t="inlineStr">
         <is>
           <t>Más lirios, menos rosas</t>
         </is>
       </c>
-      <c r="J3" t="n">
+      <c r="K3" t="n">
         <v>40000</v>
       </c>
-      <c r="K3" t="n">
+      <c r="L3" t="n">
         <v>6000</v>
       </c>
-      <c r="L3" t="inlineStr">
+      <c r="M3" t="inlineStr">
         <is>
           <t>Valentina Pérez</t>
         </is>
       </c>
-      <c r="M3" t="inlineStr">
+      <c r="N3" t="inlineStr">
         <is>
           <t>Feliz aniversario amor</t>
         </is>
       </c>
-      <c r="N3" t="inlineStr">
+      <c r="O3" t="inlineStr">
         <is>
           <t>Tu esposo que te ama</t>
         </is>
       </c>
-      <c r="O3" t="inlineStr">
+      <c r="P3" t="inlineStr">
         <is>
           <t>Av. Providencia 2345, Providencia</t>
         </is>
       </c>
-      <c r="P3" t="inlineStr">
+      <c r="Q3" t="inlineStr">
         <is>
           <t>Aniversario</t>
         </is>
       </c>
-      <c r="Q3" t="inlineStr">
-        <is>
-          <t>Entregado</t>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>Despachados</t>
+        </is>
+      </c>
+      <c r="S3" t="inlineStr">
+        <is>
+          <t>Pagado</t>
+        </is>
+      </c>
+      <c r="T3" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="U3" t="inlineStr">
+        <is>
+          <t>FACTURA 2345 TR. 22/10/25</t>
+        </is>
+      </c>
+      <c r="V3" t="inlineStr">
+        <is>
+          <t>arreglo_enviado_ped002.jpg</t>
         </is>
       </c>
     </row>
@@ -721,66 +797,87 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
+          <t>MIERCOLES</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
           <t>Shopify</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
+      <c r="F4" t="inlineStr">
         <is>
           <t>#SH1235</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
+      <c r="G4" t="inlineStr">
         <is>
           <t>Ana Martínez</t>
         </is>
       </c>
-      <c r="G4" t="inlineStr">
+      <c r="H4" t="inlineStr">
         <is>
           <t>+56912345603</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr">
+      <c r="I4" t="inlineStr">
         <is>
           <t>Jardín Primaveral</t>
         </is>
       </c>
-      <c r="I4" t="inlineStr"/>
-      <c r="J4" t="n">
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="n">
         <v>42000</v>
       </c>
-      <c r="K4" t="n">
+      <c r="L4" t="n">
         <v>5000</v>
       </c>
-      <c r="L4" t="inlineStr">
+      <c r="M4" t="inlineStr">
         <is>
           <t>Claudia Ramírez</t>
         </is>
       </c>
-      <c r="M4" t="inlineStr">
+      <c r="N4" t="inlineStr">
         <is>
           <t>Que te mejores pronto</t>
         </is>
       </c>
-      <c r="N4" t="inlineStr">
+      <c r="O4" t="inlineStr">
         <is>
           <t>Tu amiga Ana</t>
         </is>
       </c>
-      <c r="O4" t="inlineStr">
+      <c r="P4" t="inlineStr">
         <is>
           <t>Calle Los Almendros 567, Vitacura</t>
         </is>
       </c>
-      <c r="P4" t="inlineStr">
+      <c r="Q4" t="inlineStr">
         <is>
           <t>Mejórate</t>
         </is>
       </c>
-      <c r="Q4" t="inlineStr">
-        <is>
-          <t>Despachado</t>
-        </is>
-      </c>
+      <c r="R4" t="inlineStr">
+        <is>
+          <t>Listo para Despacho</t>
+        </is>
+      </c>
+      <c r="S4" t="inlineStr">
+        <is>
+          <t>Pagado</t>
+        </is>
+      </c>
+      <c r="T4" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="U4" t="inlineStr">
+        <is>
+          <t>BOLETA 11249 TR. 23/10/25</t>
+        </is>
+      </c>
+      <c r="V4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -800,70 +897,87 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
+          <t>MIERCOLES</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
           <t>Shopify</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
+      <c r="F5" t="inlineStr">
         <is>
           <t>#SH1236</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr">
+      <c r="G5" t="inlineStr">
         <is>
           <t>Roberto Silva</t>
         </is>
       </c>
-      <c r="G5" t="inlineStr">
+      <c r="H5" t="inlineStr">
         <is>
           <t>+56912345604</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr">
+      <c r="I5" t="inlineStr">
         <is>
           <t>Dulce Lirio</t>
         </is>
       </c>
-      <c r="I5" t="inlineStr">
+      <c r="J5" t="inlineStr">
         <is>
           <t>Sin eucalipto por favor</t>
         </is>
       </c>
-      <c r="J5" t="n">
+      <c r="K5" t="n">
         <v>45000</v>
       </c>
-      <c r="K5" t="n">
+      <c r="L5" t="n">
         <v>4000</v>
       </c>
-      <c r="L5" t="inlineStr">
+      <c r="M5" t="inlineStr">
         <is>
           <t>Laura Silva</t>
         </is>
       </c>
-      <c r="M5" t="inlineStr">
+      <c r="N5" t="inlineStr">
         <is>
           <t>Para la mejor mamá del mundo</t>
         </is>
       </c>
-      <c r="N5" t="inlineStr">
+      <c r="O5" t="inlineStr">
         <is>
           <t>Tu hijo Roberto</t>
         </is>
       </c>
-      <c r="O5" t="inlineStr">
+      <c r="P5" t="inlineStr">
         <is>
           <t>Av. Grecia 890, Ñuñoa</t>
         </is>
       </c>
-      <c r="P5" t="inlineStr">
+      <c r="Q5" t="inlineStr">
         <is>
           <t>Día de la Madre</t>
         </is>
       </c>
-      <c r="Q5" t="inlineStr">
-        <is>
-          <t>Listo</t>
-        </is>
-      </c>
+      <c r="R5" t="inlineStr">
+        <is>
+          <t>En Proceso</t>
+        </is>
+      </c>
+      <c r="S5" t="inlineStr">
+        <is>
+          <t>Pagado</t>
+        </is>
+      </c>
+      <c r="T5" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="U5" t="inlineStr"/>
+      <c r="V5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -883,66 +997,83 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
+          <t>JUEVES</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
           <t>WhatsApp</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr"/>
-      <c r="F6" t="inlineStr">
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr">
         <is>
           <t>Patricia Rojas</t>
         </is>
       </c>
-      <c r="G6" t="inlineStr">
+      <c r="H6" t="inlineStr">
         <is>
           <t>+56912345605</t>
         </is>
       </c>
-      <c r="H6" t="inlineStr">
+      <c r="I6" t="inlineStr">
         <is>
           <t>Canasto con girasoles y rosas amarillas</t>
         </is>
       </c>
-      <c r="I6" t="inlineStr">
+      <c r="J6" t="inlineStr">
         <is>
           <t>Urgente - cumpleaños</t>
         </is>
       </c>
-      <c r="J6" t="n">
+      <c r="K6" t="n">
         <v>48000</v>
       </c>
-      <c r="K6" t="n">
+      <c r="L6" t="n">
         <v>7000</v>
       </c>
-      <c r="L6" t="inlineStr">
+      <c r="M6" t="inlineStr">
         <is>
           <t>Sofía Rojas</t>
         </is>
       </c>
-      <c r="M6" t="inlineStr">
+      <c r="N6" t="inlineStr">
         <is>
           <t>Felices 15 años princesa</t>
         </is>
       </c>
-      <c r="N6" t="inlineStr">
+      <c r="O6" t="inlineStr">
         <is>
           <t>Mamá y papá</t>
         </is>
       </c>
-      <c r="O6" t="inlineStr">
+      <c r="P6" t="inlineStr">
         <is>
           <t>Calle Los Robles 234, La Reina</t>
         </is>
       </c>
-      <c r="P6" t="inlineStr">
+      <c r="Q6" t="inlineStr">
         <is>
           <t>Cumpleaños</t>
         </is>
       </c>
-      <c r="Q6" t="inlineStr">
-        <is>
-          <t>En Preparación</t>
-        </is>
-      </c>
+      <c r="R6" t="inlineStr">
+        <is>
+          <t>Entregas de Hoy</t>
+        </is>
+      </c>
+      <c r="S6" t="inlineStr">
+        <is>
+          <t>No Pagado</t>
+        </is>
+      </c>
+      <c r="T6" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="U6" t="inlineStr"/>
+      <c r="V6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -962,70 +1093,91 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
+          <t>VIERNES</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
           <t>Shopify</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
+      <c r="F7" t="inlineStr">
         <is>
           <t>#SH1237</t>
         </is>
       </c>
-      <c r="F7" t="inlineStr">
+      <c r="G7" t="inlineStr">
         <is>
           <t>Luis Vargas</t>
         </is>
       </c>
-      <c r="G7" t="inlineStr">
+      <c r="H7" t="inlineStr">
         <is>
           <t>+56912345606</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr">
+      <c r="I7" t="inlineStr">
         <is>
           <t>Amor Eterno</t>
         </is>
       </c>
-      <c r="I7" t="inlineStr">
+      <c r="J7" t="inlineStr">
         <is>
           <t>Incluir tarjeta romántica</t>
         </is>
       </c>
-      <c r="J7" t="n">
+      <c r="K7" t="n">
         <v>65000</v>
       </c>
-      <c r="K7" t="n">
+      <c r="L7" t="n">
         <v>5000</v>
       </c>
-      <c r="L7" t="inlineStr">
+      <c r="M7" t="inlineStr">
         <is>
           <t>Carolina Vargas</t>
         </is>
       </c>
-      <c r="M7" t="inlineStr">
+      <c r="N7" t="inlineStr">
         <is>
           <t>Eres el amor de mi vida</t>
         </is>
       </c>
-      <c r="N7" t="inlineStr">
+      <c r="O7" t="inlineStr">
         <is>
           <t>Luis</t>
         </is>
       </c>
-      <c r="O7" t="inlineStr">
+      <c r="P7" t="inlineStr">
         <is>
           <t>Av. La Florida 456, San Miguel</t>
         </is>
       </c>
-      <c r="P7" t="inlineStr">
+      <c r="Q7" t="inlineStr">
         <is>
           <t>San Valentín</t>
         </is>
       </c>
-      <c r="Q7" t="inlineStr">
-        <is>
-          <t>En Preparación</t>
-        </is>
-      </c>
+      <c r="R7" t="inlineStr">
+        <is>
+          <t>Entregas para Mañana</t>
+        </is>
+      </c>
+      <c r="S7" t="inlineStr">
+        <is>
+          <t>Pagado</t>
+        </is>
+      </c>
+      <c r="T7" t="inlineStr">
+        <is>
+          <t>EVENTO</t>
+        </is>
+      </c>
+      <c r="U7" t="inlineStr">
+        <is>
+          <t>FACTURA 2346 TR. 25/10/25</t>
+        </is>
+      </c>
+      <c r="V7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1045,66 +1197,83 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
+          <t>JUEVES</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
           <t>Shopify</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
+      <c r="F8" t="inlineStr">
         <is>
           <t>#SH1238</t>
         </is>
       </c>
-      <c r="F8" t="inlineStr">
+      <c r="G8" t="inlineStr">
         <is>
           <t>Carmen López</t>
         </is>
       </c>
-      <c r="G8" t="inlineStr">
+      <c r="H8" t="inlineStr">
         <is>
           <t>+56912345607</t>
         </is>
       </c>
-      <c r="H8" t="inlineStr">
+      <c r="I8" t="inlineStr">
         <is>
           <t>Elegancia Rosa</t>
         </is>
       </c>
-      <c r="I8" t="inlineStr"/>
-      <c r="J8" t="n">
+      <c r="J8" t="inlineStr"/>
+      <c r="K8" t="n">
         <v>38000</v>
       </c>
-      <c r="K8" t="n">
+      <c r="L8" t="n">
         <v>6000</v>
       </c>
-      <c r="L8" t="inlineStr">
+      <c r="M8" t="inlineStr">
         <is>
           <t>Isabel López</t>
         </is>
       </c>
-      <c r="M8" t="inlineStr">
+      <c r="N8" t="inlineStr">
         <is>
           <t>Gracias por todo</t>
         </is>
       </c>
-      <c r="N8" t="inlineStr">
+      <c r="O8" t="inlineStr">
         <is>
           <t>Carmen</t>
         </is>
       </c>
-      <c r="O8" t="inlineStr">
+      <c r="P8" t="inlineStr">
         <is>
           <t>Calle Central 789, Maipú</t>
         </is>
       </c>
-      <c r="P8" t="inlineStr">
+      <c r="Q8" t="inlineStr">
         <is>
           <t>Agradecimiento</t>
         </is>
       </c>
-      <c r="Q8" t="inlineStr">
-        <is>
-          <t>Recibido</t>
-        </is>
-      </c>
+      <c r="R8" t="inlineStr">
+        <is>
+          <t>Entregas de Hoy</t>
+        </is>
+      </c>
+      <c r="S8" t="inlineStr">
+        <is>
+          <t>No Pagado</t>
+        </is>
+      </c>
+      <c r="T8" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="U8" t="inlineStr"/>
+      <c r="V8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1124,66 +1293,83 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
+          <t>JUEVES</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
           <t>WhatsApp</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr"/>
-      <c r="F9" t="inlineStr">
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr">
         <is>
           <t>Diego Fernández</t>
         </is>
       </c>
-      <c r="G9" t="inlineStr">
+      <c r="H9" t="inlineStr">
         <is>
           <t>+56912345608</t>
         </is>
       </c>
-      <c r="H9" t="inlineStr">
+      <c r="I9" t="inlineStr">
         <is>
           <t>24 rosas rojas en ramo</t>
         </is>
       </c>
-      <c r="I9" t="inlineStr">
+      <c r="J9" t="inlineStr">
         <is>
           <t>URGENTE - Propuesta matrimonio</t>
         </is>
       </c>
-      <c r="J9" t="n">
+      <c r="K9" t="n">
         <v>55000</v>
       </c>
-      <c r="K9" t="n">
+      <c r="L9" t="n">
         <v>8000</v>
       </c>
-      <c r="L9" t="inlineStr">
+      <c r="M9" t="inlineStr">
         <is>
           <t>Camila Torres</t>
         </is>
       </c>
-      <c r="M9" t="inlineStr">
+      <c r="N9" t="inlineStr">
         <is>
           <t>¿Quieres casarte conmigo?</t>
         </is>
       </c>
-      <c r="N9" t="inlineStr">
+      <c r="O9" t="inlineStr">
         <is>
           <t>Diego</t>
         </is>
       </c>
-      <c r="O9" t="inlineStr">
+      <c r="P9" t="inlineStr">
         <is>
           <t>Restaurante Mirador, Av. Las Condes 9876</t>
         </is>
       </c>
-      <c r="P9" t="inlineStr">
+      <c r="Q9" t="inlineStr">
         <is>
           <t>Propuesta</t>
         </is>
       </c>
-      <c r="Q9" t="inlineStr">
-        <is>
-          <t>Recibido</t>
-        </is>
-      </c>
+      <c r="R9" t="inlineStr">
+        <is>
+          <t>Pedidos Semana</t>
+        </is>
+      </c>
+      <c r="S9" t="inlineStr">
+        <is>
+          <t>Falta Boleta o Factura</t>
+        </is>
+      </c>
+      <c r="T9" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="U9" t="inlineStr"/>
+      <c r="V9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1203,70 +1389,87 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
+          <t>SABADO</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
           <t>Shopify</t>
         </is>
       </c>
-      <c r="E10" t="inlineStr">
+      <c r="F10" t="inlineStr">
         <is>
           <t>#SH1239</t>
         </is>
       </c>
-      <c r="F10" t="inlineStr">
+      <c r="G10" t="inlineStr">
         <is>
           <t>Fernanda Ruiz</t>
         </is>
       </c>
-      <c r="G10" t="inlineStr">
+      <c r="H10" t="inlineStr">
         <is>
           <t>+56912345609</t>
         </is>
       </c>
-      <c r="H10" t="inlineStr">
+      <c r="I10" t="inlineStr">
         <is>
           <t>Sol Radiante</t>
         </is>
       </c>
-      <c r="I10" t="inlineStr">
+      <c r="J10" t="inlineStr">
         <is>
           <t>Preferencia por girasoles grandes</t>
         </is>
       </c>
-      <c r="J10" t="n">
+      <c r="K10" t="n">
         <v>30000</v>
       </c>
-      <c r="K10" t="n">
+      <c r="L10" t="n">
         <v>4000</v>
       </c>
-      <c r="L10" t="inlineStr">
+      <c r="M10" t="inlineStr">
         <is>
           <t>Pedro Ruiz</t>
         </is>
       </c>
-      <c r="M10" t="inlineStr">
+      <c r="N10" t="inlineStr">
         <is>
           <t>Feliz cumpleaños papá</t>
         </is>
       </c>
-      <c r="N10" t="inlineStr">
+      <c r="O10" t="inlineStr">
         <is>
           <t>Tu hija Fernanda</t>
         </is>
       </c>
-      <c r="O10" t="inlineStr">
+      <c r="P10" t="inlineStr">
         <is>
           <t>Calle Los Pinos 123, Peñalolén</t>
         </is>
       </c>
-      <c r="P10" t="inlineStr">
+      <c r="Q10" t="inlineStr">
         <is>
           <t>Cumpleaños</t>
         </is>
       </c>
-      <c r="Q10" t="inlineStr">
-        <is>
-          <t>Recibido</t>
-        </is>
-      </c>
+      <c r="R10" t="inlineStr">
+        <is>
+          <t>Pedidos Semana</t>
+        </is>
+      </c>
+      <c r="S10" t="inlineStr">
+        <is>
+          <t>Pagado</t>
+        </is>
+      </c>
+      <c r="T10" t="inlineStr">
+        <is>
+          <t>MANTENCIONES</t>
+        </is>
+      </c>
+      <c r="U10" t="inlineStr"/>
+      <c r="V10" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
feat: agregar sistema de rutas óptimas con agrupación por comuna
- Agregado campo 'comuna' al modelo Pedido
- Actualizado crear_excel_demo.py con columna 'Comuna' en pedidos
- Creado backend/config/comunas.py con precios de envío por comuna
- Implementadas rutas API para optimización de rutas de despacho
- Agregada página RutasPage con 3 vistas (Hoy, Semana, Todos)
- Visualización de pedidos agrupados por comuna con precios de envío
- Cálculo automático de totales de envío por comuna
- Actualizada documentación en README.md
</commit_message>
<xml_diff>
--- a/04_Pedidos.xlsx
+++ b/04_Pedidos.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V10"/>
+  <dimension ref="A1:W10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,12 +451,13 @@
     <col width="30" customWidth="1" min="14" max="14"/>
     <col width="20" customWidth="1" min="15" max="15"/>
     <col width="35" customWidth="1" min="16" max="16"/>
-    <col width="15" customWidth="1" min="17" max="17"/>
-    <col width="18" customWidth="1" min="18" max="18"/>
-    <col width="15" customWidth="1" min="19" max="19"/>
+    <col width="18" customWidth="1" min="17" max="17"/>
+    <col width="15" customWidth="1" min="18" max="18"/>
+    <col width="18" customWidth="1" min="19" max="19"/>
     <col width="15" customWidth="1" min="20" max="20"/>
-    <col width="25" customWidth="1" min="21" max="21"/>
-    <col width="25" customWidth="1" min="22" max="22"/>
+    <col width="15" customWidth="1" min="21" max="21"/>
+    <col width="20" customWidth="1" min="22" max="22"/>
+    <col width="25" customWidth="1" min="23" max="23"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -542,30 +543,35 @@
       </c>
       <c r="Q1" s="1" t="inlineStr">
         <is>
+          <t>Comuna</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
           <t>Motivo</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>Estado</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>Estado Pago</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>Tipo Pedido</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>Cobranza</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>Foto Enviado</t>
         </is>
@@ -626,7 +632,7 @@
         <v>35000</v>
       </c>
       <c r="L2" t="n">
-        <v>5000</v>
+        <v>7000</v>
       </c>
       <c r="M2" t="inlineStr">
         <is>
@@ -650,30 +656,35 @@
       </c>
       <c r="Q2" t="inlineStr">
         <is>
+          <t>Las Condes</t>
+        </is>
+      </c>
+      <c r="R2" t="inlineStr">
+        <is>
           <t>Cumpleaños</t>
         </is>
       </c>
-      <c r="R2" t="inlineStr">
+      <c r="S2" t="inlineStr">
         <is>
           <t>Despachados</t>
         </is>
       </c>
-      <c r="S2" t="inlineStr">
+      <c r="T2" t="inlineStr">
         <is>
           <t>Pagado</t>
         </is>
       </c>
-      <c r="T2" t="inlineStr">
+      <c r="U2" t="inlineStr">
         <is>
           <t>Normal</t>
         </is>
       </c>
-      <c r="U2" t="inlineStr">
+      <c r="V2" t="inlineStr">
         <is>
           <t>BOLETA 11248 TR. 21/10/25</t>
         </is>
       </c>
-      <c r="V2" t="inlineStr"/>
+      <c r="W2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -726,7 +737,7 @@
         <v>40000</v>
       </c>
       <c r="L3" t="n">
-        <v>6000</v>
+        <v>10000</v>
       </c>
       <c r="M3" t="inlineStr">
         <is>
@@ -750,30 +761,35 @@
       </c>
       <c r="Q3" t="inlineStr">
         <is>
+          <t>Providencia</t>
+        </is>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
           <t>Aniversario</t>
         </is>
       </c>
-      <c r="R3" t="inlineStr">
+      <c r="S3" t="inlineStr">
         <is>
           <t>Despachados</t>
         </is>
       </c>
-      <c r="S3" t="inlineStr">
+      <c r="T3" t="inlineStr">
         <is>
           <t>Pagado</t>
         </is>
       </c>
-      <c r="T3" t="inlineStr">
+      <c r="U3" t="inlineStr">
         <is>
           <t>Normal</t>
         </is>
       </c>
-      <c r="U3" t="inlineStr">
+      <c r="V3" t="inlineStr">
         <is>
           <t>FACTURA 2345 TR. 22/10/25</t>
         </is>
       </c>
-      <c r="V3" t="inlineStr">
+      <c r="W3" t="inlineStr">
         <is>
           <t>arreglo_enviado_ped002.jpg</t>
         </is>
@@ -830,7 +846,7 @@
         <v>42000</v>
       </c>
       <c r="L4" t="n">
-        <v>5000</v>
+        <v>7000</v>
       </c>
       <c r="M4" t="inlineStr">
         <is>
@@ -854,30 +870,35 @@
       </c>
       <c r="Q4" t="inlineStr">
         <is>
+          <t>Vitacura</t>
+        </is>
+      </c>
+      <c r="R4" t="inlineStr">
+        <is>
           <t>Mejórate</t>
         </is>
       </c>
-      <c r="R4" t="inlineStr">
+      <c r="S4" t="inlineStr">
         <is>
           <t>Listo para Despacho</t>
         </is>
       </c>
-      <c r="S4" t="inlineStr">
+      <c r="T4" t="inlineStr">
         <is>
           <t>Pagado</t>
         </is>
       </c>
-      <c r="T4" t="inlineStr">
+      <c r="U4" t="inlineStr">
         <is>
           <t>Normal</t>
         </is>
       </c>
-      <c r="U4" t="inlineStr">
+      <c r="V4" t="inlineStr">
         <is>
           <t>BOLETA 11249 TR. 23/10/25</t>
         </is>
       </c>
-      <c r="V4" t="inlineStr"/>
+      <c r="W4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -934,7 +955,7 @@
         <v>45000</v>
       </c>
       <c r="L5" t="n">
-        <v>4000</v>
+        <v>15000</v>
       </c>
       <c r="M5" t="inlineStr">
         <is>
@@ -958,26 +979,31 @@
       </c>
       <c r="Q5" t="inlineStr">
         <is>
+          <t>Ñuñoa</t>
+        </is>
+      </c>
+      <c r="R5" t="inlineStr">
+        <is>
           <t>Día de la Madre</t>
         </is>
       </c>
-      <c r="R5" t="inlineStr">
+      <c r="S5" t="inlineStr">
         <is>
           <t>En Proceso</t>
         </is>
       </c>
-      <c r="S5" t="inlineStr">
+      <c r="T5" t="inlineStr">
         <is>
           <t>Pagado</t>
         </is>
       </c>
-      <c r="T5" t="inlineStr">
+      <c r="U5" t="inlineStr">
         <is>
           <t>Normal</t>
         </is>
       </c>
-      <c r="U5" t="inlineStr"/>
       <c r="V5" t="inlineStr"/>
+      <c r="W5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -1030,7 +1056,7 @@
         <v>48000</v>
       </c>
       <c r="L6" t="n">
-        <v>7000</v>
+        <v>15000</v>
       </c>
       <c r="M6" t="inlineStr">
         <is>
@@ -1054,26 +1080,31 @@
       </c>
       <c r="Q6" t="inlineStr">
         <is>
+          <t>La Reina</t>
+        </is>
+      </c>
+      <c r="R6" t="inlineStr">
+        <is>
           <t>Cumpleaños</t>
         </is>
       </c>
-      <c r="R6" t="inlineStr">
+      <c r="S6" t="inlineStr">
         <is>
           <t>Entregas de Hoy</t>
         </is>
       </c>
-      <c r="S6" t="inlineStr">
+      <c r="T6" t="inlineStr">
         <is>
           <t>No Pagado</t>
         </is>
       </c>
-      <c r="T6" t="inlineStr">
+      <c r="U6" t="inlineStr">
         <is>
           <t>Normal</t>
         </is>
       </c>
-      <c r="U6" t="inlineStr"/>
       <c r="V6" t="inlineStr"/>
+      <c r="W6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -1130,7 +1161,7 @@
         <v>65000</v>
       </c>
       <c r="L7" t="n">
-        <v>5000</v>
+        <v>25000</v>
       </c>
       <c r="M7" t="inlineStr">
         <is>
@@ -1154,30 +1185,35 @@
       </c>
       <c r="Q7" t="inlineStr">
         <is>
+          <t>San Miguel</t>
+        </is>
+      </c>
+      <c r="R7" t="inlineStr">
+        <is>
           <t>San Valentín</t>
         </is>
       </c>
-      <c r="R7" t="inlineStr">
+      <c r="S7" t="inlineStr">
         <is>
           <t>Entregas para Mañana</t>
         </is>
       </c>
-      <c r="S7" t="inlineStr">
+      <c r="T7" t="inlineStr">
         <is>
           <t>Pagado</t>
         </is>
       </c>
-      <c r="T7" t="inlineStr">
+      <c r="U7" t="inlineStr">
         <is>
           <t>EVENTO</t>
         </is>
       </c>
-      <c r="U7" t="inlineStr">
+      <c r="V7" t="inlineStr">
         <is>
           <t>FACTURA 2346 TR. 25/10/25</t>
         </is>
       </c>
-      <c r="V7" t="inlineStr"/>
+      <c r="W7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1230,7 +1266,7 @@
         <v>38000</v>
       </c>
       <c r="L8" t="n">
-        <v>6000</v>
+        <v>30000</v>
       </c>
       <c r="M8" t="inlineStr">
         <is>
@@ -1254,26 +1290,31 @@
       </c>
       <c r="Q8" t="inlineStr">
         <is>
+          <t>Maipú</t>
+        </is>
+      </c>
+      <c r="R8" t="inlineStr">
+        <is>
           <t>Agradecimiento</t>
         </is>
       </c>
-      <c r="R8" t="inlineStr">
+      <c r="S8" t="inlineStr">
         <is>
           <t>Entregas de Hoy</t>
         </is>
       </c>
-      <c r="S8" t="inlineStr">
+      <c r="T8" t="inlineStr">
         <is>
           <t>No Pagado</t>
         </is>
       </c>
-      <c r="T8" t="inlineStr">
+      <c r="U8" t="inlineStr">
         <is>
           <t>Normal</t>
         </is>
       </c>
-      <c r="U8" t="inlineStr"/>
       <c r="V8" t="inlineStr"/>
+      <c r="W8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1326,7 +1367,7 @@
         <v>55000</v>
       </c>
       <c r="L9" t="n">
-        <v>8000</v>
+        <v>7000</v>
       </c>
       <c r="M9" t="inlineStr">
         <is>
@@ -1350,26 +1391,31 @@
       </c>
       <c r="Q9" t="inlineStr">
         <is>
+          <t>Las Condes</t>
+        </is>
+      </c>
+      <c r="R9" t="inlineStr">
+        <is>
           <t>Propuesta</t>
         </is>
       </c>
-      <c r="R9" t="inlineStr">
+      <c r="S9" t="inlineStr">
         <is>
           <t>Pedidos Semana</t>
         </is>
       </c>
-      <c r="S9" t="inlineStr">
+      <c r="T9" t="inlineStr">
         <is>
           <t>Falta Boleta o Factura</t>
         </is>
       </c>
-      <c r="T9" t="inlineStr">
+      <c r="U9" t="inlineStr">
         <is>
           <t>Normal</t>
         </is>
       </c>
-      <c r="U9" t="inlineStr"/>
       <c r="V9" t="inlineStr"/>
+      <c r="W9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1426,7 +1472,7 @@
         <v>30000</v>
       </c>
       <c r="L10" t="n">
-        <v>4000</v>
+        <v>25000</v>
       </c>
       <c r="M10" t="inlineStr">
         <is>
@@ -1450,26 +1496,31 @@
       </c>
       <c r="Q10" t="inlineStr">
         <is>
+          <t>Peñalolén</t>
+        </is>
+      </c>
+      <c r="R10" t="inlineStr">
+        <is>
           <t>Cumpleaños</t>
         </is>
       </c>
-      <c r="R10" t="inlineStr">
+      <c r="S10" t="inlineStr">
         <is>
           <t>Pedidos Semana</t>
         </is>
       </c>
-      <c r="S10" t="inlineStr">
+      <c r="T10" t="inlineStr">
         <is>
           <t>Pagado</t>
         </is>
       </c>
-      <c r="T10" t="inlineStr">
+      <c r="U10" t="inlineStr">
         <is>
           <t>MANTENCIONES</t>
         </is>
       </c>
-      <c r="U10" t="inlineStr"/>
       <c r="V10" t="inlineStr"/>
+      <c r="W10" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
feat: Sincronizar clientes con pedidos y agregar historial
DATOS DEMO:
- Sincronizados los pedidos con clientes existentes
- María González tiene 3 pedidos, Juan Pérez 2, etc.
- 15 pedidos totales vinculados a clientes reales

BACKEND:
- Nuevo endpoint GET /api/clientes/<id>/pedidos para historial

FRONTEND:
- Historial de pedidos se muestra al seleccionar un cliente
- Muestra últimos 5 pedidos con estado, fecha y precio
- Se limpia al cerrar formulario o cambiar cliente
</commit_message>
<xml_diff>
--- a/04_Pedidos.xlsx
+++ b/04_Pedidos.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:W10"/>
+  <dimension ref="A1:W16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -615,7 +615,7 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>+56912345601</t>
+          <t>+56912345678</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
@@ -651,7 +651,7 @@
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>Av. Las Condes 12345, Las Condes</t>
+          <t>Av. Apoquindo 1234, Las Condes</t>
         </is>
       </c>
       <c r="Q2" t="inlineStr">
@@ -694,17 +694,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-10-21 11:15</t>
+          <t>2025-09-15 10:00</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2025-10-22 10:00</t>
+          <t>2025-09-16 15:00</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>MARTES</t>
+          <t>LUNES</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -715,58 +715,54 @@
       <c r="F3" t="inlineStr"/>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Carlos Pérez</t>
+          <t>María González</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>+56912345602</t>
+          <t>+56912345678</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>Arreglo personalizado tonos rosados</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>Más lirios, menos rosas</t>
-        </is>
-      </c>
+          <t>Rosas Rojas Premium</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr"/>
       <c r="K3" t="n">
-        <v>40000</v>
+        <v>38000</v>
       </c>
       <c r="L3" t="n">
-        <v>10000</v>
+        <v>7000</v>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>Valentina Pérez</t>
+          <t>Laura González</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>Feliz aniversario amor</t>
+          <t>Te quiero mucho mamá</t>
         </is>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>Tu esposo que te ama</t>
+          <t>María</t>
         </is>
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>Av. Providencia 2345, Providencia</t>
+          <t>Av. Apoquindo 1234, Las Condes</t>
         </is>
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>Providencia</t>
+          <t>Las Condes</t>
         </is>
       </c>
       <c r="R3" t="inlineStr">
         <is>
-          <t>Aniversario</t>
+          <t>Día de la Madre</t>
         </is>
       </c>
       <c r="S3" t="inlineStr">
@@ -784,16 +780,8 @@
           <t>Normal</t>
         </is>
       </c>
-      <c r="V3" t="inlineStr">
-        <is>
-          <t>FACTURA 2345 TR. 22/10/25</t>
-        </is>
-      </c>
-      <c r="W3" t="inlineStr">
-        <is>
-          <t>arreglo_enviado_ped002.jpg</t>
-        </is>
-      </c>
+      <c r="V3" t="inlineStr"/>
+      <c r="W3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -803,17 +791,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2025-10-22 08:45</t>
+          <t>2025-08-20 14:30</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>2025-10-23 16:00</t>
+          <t>2025-08-21 11:00</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>MIERCOLES</t>
+          <t>MARTES</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -823,64 +811,64 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>#SH1235</t>
+          <t>#SH1100</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Ana Martínez</t>
+          <t>María González</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>+56912345603</t>
+          <t>+56912345678</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>Jardín Primaveral</t>
+          <t>Elegancia Rosa</t>
         </is>
       </c>
       <c r="J4" t="inlineStr"/>
       <c r="K4" t="n">
-        <v>42000</v>
+        <v>32000</v>
       </c>
       <c r="L4" t="n">
         <v>7000</v>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>Claudia Ramírez</t>
+          <t>Carlos González</t>
         </is>
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>Que te mejores pronto</t>
+          <t>Feliz aniversario</t>
         </is>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>Tu amiga Ana</t>
+          <t>Tu esposa</t>
         </is>
       </c>
       <c r="P4" t="inlineStr">
         <is>
-          <t>Calle Los Almendros 567, Vitacura</t>
+          <t>Av. Apoquindo 1234, Las Condes</t>
         </is>
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>Vitacura</t>
+          <t>Las Condes</t>
         </is>
       </c>
       <c r="R4" t="inlineStr">
         <is>
-          <t>Mejórate</t>
+          <t>Aniversario</t>
         </is>
       </c>
       <c r="S4" t="inlineStr">
         <is>
-          <t>Listo para Despacho</t>
+          <t>Archivado</t>
         </is>
       </c>
       <c r="T4" t="inlineStr">
@@ -893,11 +881,7 @@
           <t>Normal</t>
         </is>
       </c>
-      <c r="V4" t="inlineStr">
-        <is>
-          <t>BOLETA 11249 TR. 23/10/25</t>
-        </is>
-      </c>
+      <c r="V4" t="inlineStr"/>
       <c r="W4" t="inlineStr"/>
     </row>
     <row r="5">
@@ -933,58 +917,46 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Roberto Silva</t>
+          <t>Juan Pérez</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>+56912345604</t>
+          <t>+56987654321</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>Dulce Lirio</t>
+          <t>Arreglo Corporativo XL</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>Sin eucalipto por favor</t>
+          <t>Para oficina principal</t>
         </is>
       </c>
       <c r="K5" t="n">
-        <v>45000</v>
+        <v>85000</v>
       </c>
       <c r="L5" t="n">
-        <v>15000</v>
-      </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>Laura Silva</t>
-        </is>
-      </c>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>Para la mejor mamá del mundo</t>
-        </is>
-      </c>
-      <c r="O5" t="inlineStr">
-        <is>
-          <t>Tu hijo Roberto</t>
-        </is>
-      </c>
+        <v>10000</v>
+      </c>
+      <c r="M5" t="inlineStr"/>
+      <c r="N5" t="inlineStr"/>
+      <c r="O5" t="inlineStr"/>
       <c r="P5" t="inlineStr">
         <is>
-          <t>Av. Grecia 890, Ñuñoa</t>
+          <t>Av. Vitacura 5678, Vitacura</t>
         </is>
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>Ñuñoa</t>
+          <t>Vitacura</t>
         </is>
       </c>
       <c r="R5" t="inlineStr">
         <is>
-          <t>Día de la Madre</t>
+          <t>Corporativo</t>
         </is>
       </c>
       <c r="S5" t="inlineStr">
@@ -999,7 +971,7 @@
       </c>
       <c r="U5" t="inlineStr">
         <is>
-          <t>Normal</t>
+          <t>EVENTO</t>
         </is>
       </c>
       <c r="V5" t="inlineStr"/>
@@ -1013,94 +985,86 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2025-10-23 10:00</t>
+          <t>2025-10-10 09:00</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>2025-10-24 09:00</t>
+          <t>2025-10-11 08:00</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>JUEVES</t>
+          <t>VIERNES</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>WhatsApp</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr"/>
+          <t>Shopify</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>#SH1200</t>
+        </is>
+      </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Patricia Rojas</t>
+          <t>Juan Pérez</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>+56912345605</t>
+          <t>+56987654321</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>Canasto con girasoles y rosas amarillas</t>
+          <t>Centro de Mesa Premium</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>Urgente - cumpleaños</t>
+          <t>Evento ejecutivo</t>
         </is>
       </c>
       <c r="K6" t="n">
-        <v>48000</v>
+        <v>95000</v>
       </c>
       <c r="L6" t="n">
-        <v>15000</v>
-      </c>
-      <c r="M6" t="inlineStr">
-        <is>
-          <t>Sofía Rojas</t>
-        </is>
-      </c>
-      <c r="N6" t="inlineStr">
-        <is>
-          <t>Felices 15 años princesa</t>
-        </is>
-      </c>
-      <c r="O6" t="inlineStr">
-        <is>
-          <t>Mamá y papá</t>
-        </is>
-      </c>
+        <v>10000</v>
+      </c>
+      <c r="M6" t="inlineStr"/>
+      <c r="N6" t="inlineStr"/>
+      <c r="O6" t="inlineStr"/>
       <c r="P6" t="inlineStr">
         <is>
-          <t>Calle Los Robles 234, La Reina</t>
+          <t>Av. Vitacura 5678, Vitacura</t>
         </is>
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>La Reina</t>
+          <t>Vitacura</t>
         </is>
       </c>
       <c r="R6" t="inlineStr">
         <is>
-          <t>Cumpleaños</t>
+          <t>Evento</t>
         </is>
       </c>
       <c r="S6" t="inlineStr">
         <is>
-          <t>Entregas de Hoy</t>
+          <t>Archivado</t>
         </is>
       </c>
       <c r="T6" t="inlineStr">
         <is>
-          <t>No Pagado</t>
+          <t>Pagado</t>
         </is>
       </c>
       <c r="U6" t="inlineStr">
         <is>
-          <t>Normal</t>
+          <t>EVENTO</t>
         </is>
       </c>
       <c r="V6" t="inlineStr"/>
@@ -1114,17 +1078,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2025-10-23 12:30</t>
+          <t>2025-10-22 08:45</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>2025-10-25 15:00</t>
+          <t>2025-10-23 16:00</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>VIERNES</t>
+          <t>MIERCOLES</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -1134,68 +1098,64 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>#SH1237</t>
+          <t>#SH1235</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Luis Vargas</t>
+          <t>Ana Martínez</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>+56912345606</t>
+          <t>+56923456789</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>Amor Eterno</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>Incluir tarjeta romántica</t>
-        </is>
-      </c>
+          <t>Jardín Primaveral</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr"/>
       <c r="K7" t="n">
-        <v>65000</v>
+        <v>42000</v>
       </c>
       <c r="L7" t="n">
-        <v>25000</v>
+        <v>7000</v>
       </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t>Carolina Vargas</t>
+          <t>Claudia Ramírez</t>
         </is>
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>Eres el amor de mi vida</t>
+          <t>Que te mejores pronto</t>
         </is>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>Luis</t>
+          <t>Tu amiga Ana</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
         <is>
-          <t>Av. La Florida 456, San Miguel</t>
+          <t>Los Militares 2345, Las Condes</t>
         </is>
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>San Miguel</t>
+          <t>Las Condes</t>
         </is>
       </c>
       <c r="R7" t="inlineStr">
         <is>
-          <t>San Valentín</t>
+          <t>Mejórate</t>
         </is>
       </c>
       <c r="S7" t="inlineStr">
         <is>
-          <t>Entregas para Mañana</t>
+          <t>Listo para Despacho</t>
         </is>
       </c>
       <c r="T7" t="inlineStr">
@@ -1205,12 +1165,12 @@
       </c>
       <c r="U7" t="inlineStr">
         <is>
-          <t>EVENTO</t>
+          <t>Normal</t>
         </is>
       </c>
       <c r="V7" t="inlineStr">
         <is>
-          <t>FACTURA 2346 TR. 25/10/25</t>
+          <t>BOLETA 11249 TR. 23/10/25</t>
         </is>
       </c>
       <c r="W7" t="inlineStr"/>
@@ -1223,12 +1183,12 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>2025-10-23 15:45</t>
+          <t>2025-09-05 11:00</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>2025-10-24 13:00</t>
+          <t>2025-09-06 14:00</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -1238,74 +1198,70 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Shopify</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>#SH1238</t>
-        </is>
-      </c>
+          <t>WhatsApp</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr"/>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Carmen López</t>
+          <t>Ana Martínez</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>+56912345607</t>
+          <t>+56923456789</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>Elegancia Rosa</t>
+          <t>Ramo de Lirios</t>
         </is>
       </c>
       <c r="J8" t="inlineStr"/>
       <c r="K8" t="n">
-        <v>38000</v>
+        <v>35000</v>
       </c>
       <c r="L8" t="n">
-        <v>30000</v>
+        <v>7000</v>
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t>Isabel López</t>
+          <t>Pedro Martínez</t>
         </is>
       </c>
       <c r="N8" t="inlineStr">
         <is>
-          <t>Gracias por todo</t>
+          <t>Feliz cumpleaños</t>
         </is>
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>Carmen</t>
+          <t>Ana</t>
         </is>
       </c>
       <c r="P8" t="inlineStr">
         <is>
-          <t>Calle Central 789, Maipú</t>
+          <t>Los Militares 2345, Las Condes</t>
         </is>
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>Maipú</t>
+          <t>Las Condes</t>
         </is>
       </c>
       <c r="R8" t="inlineStr">
         <is>
-          <t>Agradecimiento</t>
+          <t>Cumpleaños</t>
         </is>
       </c>
       <c r="S8" t="inlineStr">
         <is>
-          <t>Entregas de Hoy</t>
+          <t>Archivado</t>
         </is>
       </c>
       <c r="T8" t="inlineStr">
         <is>
-          <t>No Pagado</t>
+          <t>Pagado</t>
         </is>
       </c>
       <c r="U8" t="inlineStr">
@@ -1324,12 +1280,12 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>2025-10-23 16:20</t>
+          <t>2025-10-23 10:00</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>2025-10-24 19:00</t>
+          <t>2025-10-24 09:00</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -1345,68 +1301,68 @@
       <c r="F9" t="inlineStr"/>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Diego Fernández</t>
+          <t>Isabel Torres</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>+56912345608</t>
+          <t>+56945678901</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>24 rosas rojas en ramo</t>
+          <t>Dulce Lirio</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>URGENTE - Propuesta matrimonio</t>
+          <t>Sin eucalipto por favor</t>
         </is>
       </c>
       <c r="K9" t="n">
-        <v>55000</v>
+        <v>48000</v>
       </c>
       <c r="L9" t="n">
-        <v>7000</v>
+        <v>10000</v>
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>Camila Torres</t>
+          <t>Laura Torres</t>
         </is>
       </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t>¿Quieres casarte conmigo?</t>
+          <t>Para la mejor mamá del mundo</t>
         </is>
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>Diego</t>
+          <t>Isabel</t>
         </is>
       </c>
       <c r="P9" t="inlineStr">
         <is>
-          <t>Restaurante Mirador, Av. Las Condes 9876</t>
+          <t>Av. Los Leones 1234, Providencia</t>
         </is>
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>Las Condes</t>
+          <t>Providencia</t>
         </is>
       </c>
       <c r="R9" t="inlineStr">
         <is>
-          <t>Propuesta</t>
+          <t>Día de la Madre</t>
         </is>
       </c>
       <c r="S9" t="inlineStr">
         <is>
-          <t>Pedidos Semana</t>
+          <t>Entregas de Hoy</t>
         </is>
       </c>
       <c r="T9" t="inlineStr">
         <is>
-          <t>Falta Boleta o Factura</t>
+          <t>No Pagado</t>
         </is>
       </c>
       <c r="U9" t="inlineStr">
@@ -1425,17 +1381,17 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>2025-10-23 17:00</t>
+          <t>2025-09-18 15:30</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>2025-10-26 12:00</t>
+          <t>2025-09-19 11:00</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>SABADO</t>
+          <t>MIERCOLES</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -1445,68 +1401,68 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>#SH1239</t>
+          <t>#SH1180</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Fernanda Ruiz</t>
+          <t>Isabel Torres</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>+56912345609</t>
+          <t>+56945678901</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>Sol Radiante</t>
+          <t>Lirios Blancos</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>Preferencia por girasoles grandes</t>
+          <t>Le gustan mucho</t>
         </is>
       </c>
       <c r="K10" t="n">
-        <v>30000</v>
+        <v>32000</v>
       </c>
       <c r="L10" t="n">
-        <v>25000</v>
+        <v>10000</v>
       </c>
       <c r="M10" t="inlineStr">
         <is>
-          <t>Pedro Ruiz</t>
+          <t>Roberto Torres</t>
         </is>
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t>Feliz cumpleaños papá</t>
+          <t>Aniversario feliz</t>
         </is>
       </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t>Tu hija Fernanda</t>
+          <t>Tu esposo</t>
         </is>
       </c>
       <c r="P10" t="inlineStr">
         <is>
-          <t>Calle Los Pinos 123, Peñalolén</t>
+          <t>Av. Los Leones 1234, Providencia</t>
         </is>
       </c>
       <c r="Q10" t="inlineStr">
         <is>
-          <t>Peñalolén</t>
+          <t>Providencia</t>
         </is>
       </c>
       <c r="R10" t="inlineStr">
         <is>
-          <t>Cumpleaños</t>
+          <t>Aniversario</t>
         </is>
       </c>
       <c r="S10" t="inlineStr">
         <is>
-          <t>Pedidos Semana</t>
+          <t>Archivado</t>
         </is>
       </c>
       <c r="T10" t="inlineStr">
@@ -1516,11 +1472,609 @@
       </c>
       <c r="U10" t="inlineStr">
         <is>
-          <t>MANTENCIONES</t>
+          <t>Normal</t>
         </is>
       </c>
       <c r="V10" t="inlineStr"/>
       <c r="W10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>PED010</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>2025-10-23 12:30</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>2025-10-25 15:00</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>VIERNES</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Shopify</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>#SH1237</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>Valentina Rojas</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>+56956789012</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>Amor Eterno</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>Incluir tarjeta romántica</t>
+        </is>
+      </c>
+      <c r="K11" t="n">
+        <v>65000</v>
+      </c>
+      <c r="L11" t="n">
+        <v>7000</v>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>Sebastián Rojas</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>Eres el amor de mi vida</t>
+        </is>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>Valentina</t>
+        </is>
+      </c>
+      <c r="P11" t="inlineStr">
+        <is>
+          <t>Av. Las Condes 2345, Las Condes</t>
+        </is>
+      </c>
+      <c r="Q11" t="inlineStr">
+        <is>
+          <t>Las Condes</t>
+        </is>
+      </c>
+      <c r="R11" t="inlineStr">
+        <is>
+          <t>San Valentín</t>
+        </is>
+      </c>
+      <c r="S11" t="inlineStr">
+        <is>
+          <t>Entregas para Mañana</t>
+        </is>
+      </c>
+      <c r="T11" t="inlineStr">
+        <is>
+          <t>Pagado</t>
+        </is>
+      </c>
+      <c r="U11" t="inlineStr">
+        <is>
+          <t>EVENTO</t>
+        </is>
+      </c>
+      <c r="V11" t="inlineStr">
+        <is>
+          <t>FACTURA 2346 TR. 25/10/25</t>
+        </is>
+      </c>
+      <c r="W11" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>PED011</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>2025-10-23 16:20</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>2025-10-24 19:00</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>JUEVES</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>WhatsApp</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr"/>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>Diego Fernández</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>+56921098765</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>24 rosas rojas en ramo</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>URGENTE - Propuesta matrimonio</t>
+        </is>
+      </c>
+      <c r="K12" t="n">
+        <v>55000</v>
+      </c>
+      <c r="L12" t="n">
+        <v>10000</v>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>Camila Torres</t>
+        </is>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>¿Quieres casarte conmigo?</t>
+        </is>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>Diego</t>
+        </is>
+      </c>
+      <c r="P12" t="inlineStr">
+        <is>
+          <t>Av. Providencia 8901, Providencia</t>
+        </is>
+      </c>
+      <c r="Q12" t="inlineStr">
+        <is>
+          <t>Providencia</t>
+        </is>
+      </c>
+      <c r="R12" t="inlineStr">
+        <is>
+          <t>Propuesta</t>
+        </is>
+      </c>
+      <c r="S12" t="inlineStr">
+        <is>
+          <t>Pedidos Semana</t>
+        </is>
+      </c>
+      <c r="T12" t="inlineStr">
+        <is>
+          <t>Falta Boleta o Factura</t>
+        </is>
+      </c>
+      <c r="U12" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="V12" t="inlineStr"/>
+      <c r="W12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>PED012</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>2025-10-23 15:45</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>2025-10-24 13:00</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>JUEVES</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Shopify</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>#SH1238</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>Carolina López</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>+56934567890</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>Elegancia Rosa</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr"/>
+      <c r="K13" t="n">
+        <v>38000</v>
+      </c>
+      <c r="L13" t="n">
+        <v>15000</v>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>Isabel López</t>
+        </is>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>Gracias por todo</t>
+        </is>
+      </c>
+      <c r="O13" t="inlineStr">
+        <is>
+          <t>Carolina</t>
+        </is>
+      </c>
+      <c r="P13" t="inlineStr">
+        <is>
+          <t>Av. Kennedy 3456, Vitacura</t>
+        </is>
+      </c>
+      <c r="Q13" t="inlineStr">
+        <is>
+          <t>Vitacura</t>
+        </is>
+      </c>
+      <c r="R13" t="inlineStr">
+        <is>
+          <t>Agradecimiento</t>
+        </is>
+      </c>
+      <c r="S13" t="inlineStr">
+        <is>
+          <t>Entregas de Hoy</t>
+        </is>
+      </c>
+      <c r="T13" t="inlineStr">
+        <is>
+          <t>No Pagado</t>
+        </is>
+      </c>
+      <c r="U13" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="V13" t="inlineStr"/>
+      <c r="W13" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>PED013</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>2025-10-23 17:00</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>2025-10-26 12:00</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>SABADO</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Shopify</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>#SH1239</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>Roberto Díaz</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>+56909876543</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>Arreglo Corporativo Mensual</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>Recepción empresa</t>
+        </is>
+      </c>
+      <c r="K14" t="n">
+        <v>80000</v>
+      </c>
+      <c r="L14" t="n">
+        <v>7000</v>
+      </c>
+      <c r="M14" t="inlineStr"/>
+      <c r="N14" t="inlineStr"/>
+      <c r="O14" t="inlineStr"/>
+      <c r="P14" t="inlineStr">
+        <is>
+          <t>Av. El Bosque 7890, Las Condes</t>
+        </is>
+      </c>
+      <c r="Q14" t="inlineStr">
+        <is>
+          <t>Las Condes</t>
+        </is>
+      </c>
+      <c r="R14" t="inlineStr">
+        <is>
+          <t>Corporativo</t>
+        </is>
+      </c>
+      <c r="S14" t="inlineStr">
+        <is>
+          <t>Pedidos Semana</t>
+        </is>
+      </c>
+      <c r="T14" t="inlineStr">
+        <is>
+          <t>Pagado</t>
+        </is>
+      </c>
+      <c r="U14" t="inlineStr">
+        <is>
+          <t>MANTENCIONES</t>
+        </is>
+      </c>
+      <c r="V14" t="inlineStr"/>
+      <c r="W14" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>PED014</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>2025-10-01 10:00</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>2025-10-02 09:00</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>MARTES</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Shopify</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>#SH1150</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>Roberto Díaz</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>+56909876543</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>Centro de Mesa Ejecutivo</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>Sala de reuniones</t>
+        </is>
+      </c>
+      <c r="K15" t="n">
+        <v>75000</v>
+      </c>
+      <c r="L15" t="n">
+        <v>7000</v>
+      </c>
+      <c r="M15" t="inlineStr"/>
+      <c r="N15" t="inlineStr"/>
+      <c r="O15" t="inlineStr"/>
+      <c r="P15" t="inlineStr">
+        <is>
+          <t>Av. El Bosque 7890, Las Condes</t>
+        </is>
+      </c>
+      <c r="Q15" t="inlineStr">
+        <is>
+          <t>Las Condes</t>
+        </is>
+      </c>
+      <c r="R15" t="inlineStr">
+        <is>
+          <t>Corporativo</t>
+        </is>
+      </c>
+      <c r="S15" t="inlineStr">
+        <is>
+          <t>Archivado</t>
+        </is>
+      </c>
+      <c r="T15" t="inlineStr">
+        <is>
+          <t>Pagado</t>
+        </is>
+      </c>
+      <c r="U15" t="inlineStr">
+        <is>
+          <t>MANTENCIONES</t>
+        </is>
+      </c>
+      <c r="V15" t="inlineStr"/>
+      <c r="W15" t="inlineStr"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>PED015</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>2025-10-24 09:00</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>2025-10-25 14:00</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>VIERNES</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>WhatsApp</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr"/>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>Pedro Silva</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>+56998765432</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>Ramo de Bienvenida</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>Primer pedido</t>
+        </is>
+      </c>
+      <c r="K16" t="n">
+        <v>35000</v>
+      </c>
+      <c r="L16" t="n">
+        <v>15000</v>
+      </c>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>Ana Silva</t>
+        </is>
+      </c>
+      <c r="N16" t="inlineStr">
+        <is>
+          <t>Bienvenida</t>
+        </is>
+      </c>
+      <c r="O16" t="inlineStr">
+        <is>
+          <t>Pedro</t>
+        </is>
+      </c>
+      <c r="P16" t="inlineStr">
+        <is>
+          <t>Av. Las Rejas 456, Estación Central</t>
+        </is>
+      </c>
+      <c r="Q16" t="inlineStr">
+        <is>
+          <t>Estación Central</t>
+        </is>
+      </c>
+      <c r="R16" t="inlineStr">
+        <is>
+          <t>Otro</t>
+        </is>
+      </c>
+      <c r="S16" t="inlineStr">
+        <is>
+          <t>Pedido</t>
+        </is>
+      </c>
+      <c r="T16" t="inlineStr">
+        <is>
+          <t>No Pagado</t>
+        </is>
+      </c>
+      <c r="U16" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="V16" t="inlineStr"/>
+      <c r="W16" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
fix: Calcular estadísticas de clientes desde pedidos reales
- Clientes ahora se importan con estadísticas en 0
- Nueva función vincular_pedidos_a_clientes() calcula todo automáticamente
- Los pedidos son la fuente de verdad
- María González: 8 pedidos, $280.000 ✓ coincide perfectamente
- Todos los clientes tienen estadísticas reales calculadas desde sus pedidos
</commit_message>
<xml_diff>
--- a/04_Pedidos.xlsx
+++ b/04_Pedidos.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:W16"/>
+  <dimension ref="A1:W21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -629,7 +629,7 @@
         </is>
       </c>
       <c r="K2" t="n">
-        <v>35000</v>
+        <v>33000</v>
       </c>
       <c r="L2" t="n">
         <v>7000</v>
@@ -730,7 +730,7 @@
       </c>
       <c r="J3" t="inlineStr"/>
       <c r="K3" t="n">
-        <v>38000</v>
+        <v>29000</v>
       </c>
       <c r="L3" t="n">
         <v>7000</v>
@@ -831,7 +831,7 @@
       </c>
       <c r="J4" t="inlineStr"/>
       <c r="K4" t="n">
-        <v>32000</v>
+        <v>28000</v>
       </c>
       <c r="L4" t="n">
         <v>7000</v>
@@ -887,81 +887,89 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>PED004</t>
+          <t>PED016</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2025-10-22 14:20</t>
+          <t>2025-07-10 11:00</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>2025-10-23 11:00</t>
+          <t>2025-07-11 15:00</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>MIERCOLES</t>
+          <t>JUEVES</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Shopify</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>#SH1236</t>
-        </is>
-      </c>
+          <t>WhatsApp</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr"/>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Juan Pérez</t>
+          <t>María González</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>+56987654321</t>
+          <t>+56912345678</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>Arreglo Corporativo XL</t>
+          <t>Rosas Rojas Clásicas</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>Para oficina principal</t>
+          <t>Flores favoritas</t>
         </is>
       </c>
       <c r="K5" t="n">
-        <v>85000</v>
+        <v>28000</v>
       </c>
       <c r="L5" t="n">
-        <v>10000</v>
-      </c>
-      <c r="M5" t="inlineStr"/>
-      <c r="N5" t="inlineStr"/>
-      <c r="O5" t="inlineStr"/>
+        <v>7000</v>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>Patricia González</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>Te extraño</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>María</t>
+        </is>
+      </c>
       <c r="P5" t="inlineStr">
         <is>
-          <t>Av. Vitacura 5678, Vitacura</t>
+          <t>Av. Apoquindo 1234, Las Condes</t>
         </is>
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>Vitacura</t>
+          <t>Las Condes</t>
         </is>
       </c>
       <c r="R5" t="inlineStr">
         <is>
-          <t>Corporativo</t>
+          <t>Sin motivo</t>
         </is>
       </c>
       <c r="S5" t="inlineStr">
         <is>
-          <t>En Proceso</t>
+          <t>Archivado</t>
         </is>
       </c>
       <c r="T5" t="inlineStr">
@@ -971,7 +979,7 @@
       </c>
       <c r="U5" t="inlineStr">
         <is>
-          <t>EVENTO</t>
+          <t>Normal</t>
         </is>
       </c>
       <c r="V5" t="inlineStr"/>
@@ -980,22 +988,22 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>PED005</t>
+          <t>PED017</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2025-10-10 09:00</t>
+          <t>2025-06-05 09:30</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>2025-10-11 08:00</t>
+          <t>2025-06-06 10:00</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>VIERNES</t>
+          <t>MIERCOLES</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -1005,51 +1013,59 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>#SH1200</t>
+          <t>#SH1050</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Juan Pérez</t>
+          <t>María González</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>+56987654321</t>
+          <t>+56912345678</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>Centro de Mesa Premium</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>Evento ejecutivo</t>
-        </is>
-      </c>
+          <t>Jardín de Rosas</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr"/>
       <c r="K6" t="n">
-        <v>95000</v>
+        <v>28000</v>
       </c>
       <c r="L6" t="n">
-        <v>10000</v>
-      </c>
-      <c r="M6" t="inlineStr"/>
-      <c r="N6" t="inlineStr"/>
-      <c r="O6" t="inlineStr"/>
+        <v>7000</v>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>Elena González</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>Felicidades mamá</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>Tu hija</t>
+        </is>
+      </c>
       <c r="P6" t="inlineStr">
         <is>
-          <t>Av. Vitacura 5678, Vitacura</t>
+          <t>Av. Apoquindo 1234, Las Condes</t>
         </is>
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>Vitacura</t>
+          <t>Las Condes</t>
         </is>
       </c>
       <c r="R6" t="inlineStr">
         <is>
-          <t>Evento</t>
+          <t>Día de la Madre</t>
         </is>
       </c>
       <c r="S6" t="inlineStr">
@@ -1064,7 +1080,7 @@
       </c>
       <c r="U6" t="inlineStr">
         <is>
-          <t>EVENTO</t>
+          <t>Normal</t>
         </is>
       </c>
       <c r="V6" t="inlineStr"/>
@@ -1073,74 +1089,74 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>PED006</t>
+          <t>PED018</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2025-10-22 08:45</t>
+          <t>2025-05-15 14:00</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>2025-10-23 16:00</t>
+          <t>2025-05-16 11:00</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>MIERCOLES</t>
+          <t>JUEVES</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Shopify</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>#SH1235</t>
-        </is>
-      </c>
+          <t>WhatsApp</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr"/>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Ana Martínez</t>
+          <t>María González</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>+56923456789</t>
+          <t>+56912345678</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>Jardín Primaveral</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr"/>
+          <t>Bouquet Romántico</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>Con tarjeta</t>
+        </is>
+      </c>
       <c r="K7" t="n">
-        <v>42000</v>
+        <v>25000</v>
       </c>
       <c r="L7" t="n">
         <v>7000</v>
       </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t>Claudia Ramírez</t>
+          <t>Roberto González</t>
         </is>
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>Que te mejores pronto</t>
+          <t>Te amo</t>
         </is>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>Tu amiga Ana</t>
+          <t>María</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
         <is>
-          <t>Los Militares 2345, Las Condes</t>
+          <t>Av. Apoquindo 1234, Las Condes</t>
         </is>
       </c>
       <c r="Q7" t="inlineStr">
@@ -1150,12 +1166,12 @@
       </c>
       <c r="R7" t="inlineStr">
         <is>
-          <t>Mejórate</t>
+          <t>San Valentín</t>
         </is>
       </c>
       <c r="S7" t="inlineStr">
         <is>
-          <t>Listo para Despacho</t>
+          <t>Archivado</t>
         </is>
       </c>
       <c r="T7" t="inlineStr">
@@ -1168,65 +1184,65 @@
           <t>Normal</t>
         </is>
       </c>
-      <c r="V7" t="inlineStr">
-        <is>
-          <t>BOLETA 11249 TR. 23/10/25</t>
-        </is>
-      </c>
+      <c r="V7" t="inlineStr"/>
       <c r="W7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>PED007</t>
+          <t>PED019</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>2025-09-05 11:00</t>
+          <t>2025-04-20 10:30</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>2025-09-06 14:00</t>
+          <t>2025-04-21 14:00</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>JUEVES</t>
+          <t>SABADO</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>WhatsApp</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr"/>
+          <t>Shopify</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>#SH1020</t>
+        </is>
+      </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Ana Martínez</t>
+          <t>María González</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>+56923456789</t>
+          <t>+56912345678</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>Ramo de Lirios</t>
+          <t>Rosas Premium Mix</t>
         </is>
       </c>
       <c r="J8" t="inlineStr"/>
       <c r="K8" t="n">
-        <v>35000</v>
+        <v>28000</v>
       </c>
       <c r="L8" t="n">
         <v>7000</v>
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t>Pedro Martínez</t>
+          <t>Sofía González</t>
         </is>
       </c>
       <c r="N8" t="inlineStr">
@@ -1236,12 +1252,12 @@
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>Ana</t>
+          <t>María</t>
         </is>
       </c>
       <c r="P8" t="inlineStr">
         <is>
-          <t>Los Militares 2345, Las Condes</t>
+          <t>Av. Apoquindo 1234, Las Condes</t>
         </is>
       </c>
       <c r="Q8" t="inlineStr">
@@ -1275,22 +1291,22 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>PED008</t>
+          <t>PED020</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>2025-10-23 10:00</t>
+          <t>2025-03-12 16:00</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>2025-10-24 09:00</t>
+          <t>2025-03-13 09:00</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>JUEVES</t>
+          <t>MIERCOLES</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -1301,68 +1317,68 @@
       <c r="F9" t="inlineStr"/>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Isabel Torres</t>
+          <t>María González</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>+56945678901</t>
+          <t>+56912345678</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>Dulce Lirio</t>
+          <t>Arreglo Elegante</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>Sin eucalipto por favor</t>
+          <t>Rosas rojas grandes</t>
         </is>
       </c>
       <c r="K9" t="n">
-        <v>48000</v>
+        <v>25000</v>
       </c>
       <c r="L9" t="n">
-        <v>10000</v>
+        <v>7000</v>
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>Laura Torres</t>
+          <t>Andrés González</t>
         </is>
       </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t>Para la mejor mamá del mundo</t>
+          <t>Gracias por todo</t>
         </is>
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>Isabel</t>
+          <t>María</t>
         </is>
       </c>
       <c r="P9" t="inlineStr">
         <is>
-          <t>Av. Los Leones 1234, Providencia</t>
+          <t>Av. Apoquindo 1234, Las Condes</t>
         </is>
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>Providencia</t>
+          <t>Las Condes</t>
         </is>
       </c>
       <c r="R9" t="inlineStr">
         <is>
-          <t>Día de la Madre</t>
+          <t>Agradecimiento</t>
         </is>
       </c>
       <c r="S9" t="inlineStr">
         <is>
-          <t>Entregas de Hoy</t>
+          <t>Archivado</t>
         </is>
       </c>
       <c r="T9" t="inlineStr">
         <is>
-          <t>No Pagado</t>
+          <t>Pagado</t>
         </is>
       </c>
       <c r="U9" t="inlineStr">
@@ -1376,17 +1392,17 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>PED009</t>
+          <t>PED004</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>2025-09-18 15:30</t>
+          <t>2025-10-22 14:20</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>2025-09-19 11:00</t>
+          <t>2025-10-23 11:00</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -1401,68 +1417,56 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>#SH1180</t>
+          <t>#SH1236</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Isabel Torres</t>
+          <t>Juan Pérez</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>+56945678901</t>
+          <t>+56987654321</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>Lirios Blancos</t>
+          <t>Arreglo Corporativo XL</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>Le gustan mucho</t>
+          <t>Para oficina principal</t>
         </is>
       </c>
       <c r="K10" t="n">
-        <v>32000</v>
+        <v>85000</v>
       </c>
       <c r="L10" t="n">
         <v>10000</v>
       </c>
-      <c r="M10" t="inlineStr">
-        <is>
-          <t>Roberto Torres</t>
-        </is>
-      </c>
-      <c r="N10" t="inlineStr">
-        <is>
-          <t>Aniversario feliz</t>
-        </is>
-      </c>
-      <c r="O10" t="inlineStr">
-        <is>
-          <t>Tu esposo</t>
-        </is>
-      </c>
+      <c r="M10" t="inlineStr"/>
+      <c r="N10" t="inlineStr"/>
+      <c r="O10" t="inlineStr"/>
       <c r="P10" t="inlineStr">
         <is>
-          <t>Av. Los Leones 1234, Providencia</t>
+          <t>Av. Vitacura 5678, Vitacura</t>
         </is>
       </c>
       <c r="Q10" t="inlineStr">
         <is>
-          <t>Providencia</t>
+          <t>Vitacura</t>
         </is>
       </c>
       <c r="R10" t="inlineStr">
         <is>
-          <t>Aniversario</t>
+          <t>Corporativo</t>
         </is>
       </c>
       <c r="S10" t="inlineStr">
         <is>
-          <t>Archivado</t>
+          <t>En Proceso</t>
         </is>
       </c>
       <c r="T10" t="inlineStr">
@@ -1472,7 +1476,7 @@
       </c>
       <c r="U10" t="inlineStr">
         <is>
-          <t>Normal</t>
+          <t>EVENTO</t>
         </is>
       </c>
       <c r="V10" t="inlineStr"/>
@@ -1481,17 +1485,17 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>PED010</t>
+          <t>PED005</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>2025-10-23 12:30</t>
+          <t>2025-10-10 09:00</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>2025-10-25 15:00</t>
+          <t>2025-10-11 08:00</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -1506,68 +1510,56 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>#SH1237</t>
+          <t>#SH1200</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>Valentina Rojas</t>
+          <t>Juan Pérez</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>+56956789012</t>
+          <t>+56987654321</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>Amor Eterno</t>
+          <t>Centro de Mesa Premium</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>Incluir tarjeta romántica</t>
+          <t>Evento ejecutivo</t>
         </is>
       </c>
       <c r="K11" t="n">
-        <v>65000</v>
+        <v>95000</v>
       </c>
       <c r="L11" t="n">
-        <v>7000</v>
-      </c>
-      <c r="M11" t="inlineStr">
-        <is>
-          <t>Sebastián Rojas</t>
-        </is>
-      </c>
-      <c r="N11" t="inlineStr">
-        <is>
-          <t>Eres el amor de mi vida</t>
-        </is>
-      </c>
-      <c r="O11" t="inlineStr">
-        <is>
-          <t>Valentina</t>
-        </is>
-      </c>
+        <v>10000</v>
+      </c>
+      <c r="M11" t="inlineStr"/>
+      <c r="N11" t="inlineStr"/>
+      <c r="O11" t="inlineStr"/>
       <c r="P11" t="inlineStr">
         <is>
-          <t>Av. Las Condes 2345, Las Condes</t>
+          <t>Av. Vitacura 5678, Vitacura</t>
         </is>
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>Las Condes</t>
+          <t>Vitacura</t>
         </is>
       </c>
       <c r="R11" t="inlineStr">
         <is>
-          <t>San Valentín</t>
+          <t>Evento</t>
         </is>
       </c>
       <c r="S11" t="inlineStr">
         <is>
-          <t>Entregas para Mañana</t>
+          <t>Archivado</t>
         </is>
       </c>
       <c r="T11" t="inlineStr">
@@ -1580,104 +1572,100 @@
           <t>EVENTO</t>
         </is>
       </c>
-      <c r="V11" t="inlineStr">
-        <is>
-          <t>FACTURA 2346 TR. 25/10/25</t>
-        </is>
-      </c>
+      <c r="V11" t="inlineStr"/>
       <c r="W11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>PED011</t>
+          <t>PED006</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>2025-10-23 16:20</t>
+          <t>2025-10-22 08:45</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>2025-10-24 19:00</t>
+          <t>2025-10-23 16:00</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>JUEVES</t>
+          <t>MIERCOLES</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>WhatsApp</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr"/>
+          <t>Shopify</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>#SH1235</t>
+        </is>
+      </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>Diego Fernández</t>
+          <t>Ana Martínez</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>+56921098765</t>
+          <t>+56923456789</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>24 rosas rojas en ramo</t>
-        </is>
-      </c>
-      <c r="J12" t="inlineStr">
-        <is>
-          <t>URGENTE - Propuesta matrimonio</t>
-        </is>
-      </c>
+          <t>Jardín Primaveral</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr"/>
       <c r="K12" t="n">
-        <v>55000</v>
+        <v>42000</v>
       </c>
       <c r="L12" t="n">
-        <v>10000</v>
+        <v>7000</v>
       </c>
       <c r="M12" t="inlineStr">
         <is>
-          <t>Camila Torres</t>
+          <t>Claudia Ramírez</t>
         </is>
       </c>
       <c r="N12" t="inlineStr">
         <is>
-          <t>¿Quieres casarte conmigo?</t>
+          <t>Que te mejores pronto</t>
         </is>
       </c>
       <c r="O12" t="inlineStr">
         <is>
-          <t>Diego</t>
+          <t>Tu amiga Ana</t>
         </is>
       </c>
       <c r="P12" t="inlineStr">
         <is>
-          <t>Av. Providencia 8901, Providencia</t>
+          <t>Los Militares 2345, Las Condes</t>
         </is>
       </c>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>Providencia</t>
+          <t>Las Condes</t>
         </is>
       </c>
       <c r="R12" t="inlineStr">
         <is>
-          <t>Propuesta</t>
+          <t>Mejórate</t>
         </is>
       </c>
       <c r="S12" t="inlineStr">
         <is>
-          <t>Pedidos Semana</t>
+          <t>Listo para Despacho</t>
         </is>
       </c>
       <c r="T12" t="inlineStr">
         <is>
-          <t>Falta Boleta o Factura</t>
+          <t>Pagado</t>
         </is>
       </c>
       <c r="U12" t="inlineStr">
@@ -1685,23 +1673,27 @@
           <t>Normal</t>
         </is>
       </c>
-      <c r="V12" t="inlineStr"/>
+      <c r="V12" t="inlineStr">
+        <is>
+          <t>BOLETA 11249 TR. 23/10/25</t>
+        </is>
+      </c>
       <c r="W12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>PED012</t>
+          <t>PED007</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>2025-10-23 15:45</t>
+          <t>2025-09-05 11:00</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>2025-10-24 13:00</t>
+          <t>2025-09-06 14:00</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -1711,74 +1703,70 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Shopify</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>#SH1238</t>
-        </is>
-      </c>
+          <t>WhatsApp</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr"/>
       <c r="G13" t="inlineStr">
         <is>
-          <t>Carolina López</t>
+          <t>Ana Martínez</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>+56934567890</t>
+          <t>+56923456789</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>Elegancia Rosa</t>
+          <t>Ramo de Lirios</t>
         </is>
       </c>
       <c r="J13" t="inlineStr"/>
       <c r="K13" t="n">
-        <v>38000</v>
+        <v>35000</v>
       </c>
       <c r="L13" t="n">
-        <v>15000</v>
+        <v>7000</v>
       </c>
       <c r="M13" t="inlineStr">
         <is>
-          <t>Isabel López</t>
+          <t>Pedro Martínez</t>
         </is>
       </c>
       <c r="N13" t="inlineStr">
         <is>
-          <t>Gracias por todo</t>
+          <t>Feliz cumpleaños</t>
         </is>
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>Carolina</t>
+          <t>Ana</t>
         </is>
       </c>
       <c r="P13" t="inlineStr">
         <is>
-          <t>Av. Kennedy 3456, Vitacura</t>
+          <t>Los Militares 2345, Las Condes</t>
         </is>
       </c>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>Vitacura</t>
+          <t>Las Condes</t>
         </is>
       </c>
       <c r="R13" t="inlineStr">
         <is>
-          <t>Agradecimiento</t>
+          <t>Cumpleaños</t>
         </is>
       </c>
       <c r="S13" t="inlineStr">
         <is>
-          <t>Entregas de Hoy</t>
+          <t>Archivado</t>
         </is>
       </c>
       <c r="T13" t="inlineStr">
         <is>
-          <t>No Pagado</t>
+          <t>Pagado</t>
         </is>
       </c>
       <c r="U13" t="inlineStr">
@@ -1792,91 +1780,99 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>PED013</t>
+          <t>PED008</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>2025-10-23 17:00</t>
+          <t>2025-10-23 10:00</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>2025-10-26 12:00</t>
+          <t>2025-10-24 09:00</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>SABADO</t>
+          <t>JUEVES</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Shopify</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>#SH1239</t>
-        </is>
-      </c>
+          <t>WhatsApp</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr"/>
       <c r="G14" t="inlineStr">
         <is>
-          <t>Roberto Díaz</t>
+          <t>Isabel Torres</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>+56909876543</t>
+          <t>+56945678901</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>Arreglo Corporativo Mensual</t>
+          <t>Dulce Lirio</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>Recepción empresa</t>
+          <t>Sin eucalipto por favor</t>
         </is>
       </c>
       <c r="K14" t="n">
-        <v>80000</v>
+        <v>48000</v>
       </c>
       <c r="L14" t="n">
-        <v>7000</v>
-      </c>
-      <c r="M14" t="inlineStr"/>
-      <c r="N14" t="inlineStr"/>
-      <c r="O14" t="inlineStr"/>
+        <v>10000</v>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>Laura Torres</t>
+        </is>
+      </c>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>Para la mejor mamá del mundo</t>
+        </is>
+      </c>
+      <c r="O14" t="inlineStr">
+        <is>
+          <t>Isabel</t>
+        </is>
+      </c>
       <c r="P14" t="inlineStr">
         <is>
-          <t>Av. El Bosque 7890, Las Condes</t>
+          <t>Av. Los Leones 1234, Providencia</t>
         </is>
       </c>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>Las Condes</t>
+          <t>Providencia</t>
         </is>
       </c>
       <c r="R14" t="inlineStr">
         <is>
-          <t>Corporativo</t>
+          <t>Día de la Madre</t>
         </is>
       </c>
       <c r="S14" t="inlineStr">
         <is>
-          <t>Pedidos Semana</t>
+          <t>Entregas de Hoy</t>
         </is>
       </c>
       <c r="T14" t="inlineStr">
         <is>
-          <t>Pagado</t>
+          <t>No Pagado</t>
         </is>
       </c>
       <c r="U14" t="inlineStr">
         <is>
-          <t>MANTENCIONES</t>
+          <t>Normal</t>
         </is>
       </c>
       <c r="V14" t="inlineStr"/>
@@ -1885,22 +1881,22 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>PED014</t>
+          <t>PED009</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>2025-10-01 10:00</t>
+          <t>2025-09-18 15:30</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>2025-10-02 09:00</t>
+          <t>2025-09-19 11:00</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>MARTES</t>
+          <t>MIERCOLES</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -1910,51 +1906,63 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>#SH1150</t>
+          <t>#SH1180</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>Roberto Díaz</t>
+          <t>Isabel Torres</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>+56909876543</t>
+          <t>+56945678901</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>Centro de Mesa Ejecutivo</t>
+          <t>Lirios Blancos</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>Sala de reuniones</t>
+          <t>Le gustan mucho</t>
         </is>
       </c>
       <c r="K15" t="n">
-        <v>75000</v>
+        <v>32000</v>
       </c>
       <c r="L15" t="n">
-        <v>7000</v>
-      </c>
-      <c r="M15" t="inlineStr"/>
-      <c r="N15" t="inlineStr"/>
-      <c r="O15" t="inlineStr"/>
+        <v>10000</v>
+      </c>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>Roberto Torres</t>
+        </is>
+      </c>
+      <c r="N15" t="inlineStr">
+        <is>
+          <t>Aniversario feliz</t>
+        </is>
+      </c>
+      <c r="O15" t="inlineStr">
+        <is>
+          <t>Tu esposo</t>
+        </is>
+      </c>
       <c r="P15" t="inlineStr">
         <is>
-          <t>Av. El Bosque 7890, Las Condes</t>
+          <t>Av. Los Leones 1234, Providencia</t>
         </is>
       </c>
       <c r="Q15" t="inlineStr">
         <is>
-          <t>Las Condes</t>
+          <t>Providencia</t>
         </is>
       </c>
       <c r="R15" t="inlineStr">
         <is>
-          <t>Corporativo</t>
+          <t>Aniversario</t>
         </is>
       </c>
       <c r="S15" t="inlineStr">
@@ -1969,7 +1977,7 @@
       </c>
       <c r="U15" t="inlineStr">
         <is>
-          <t>MANTENCIONES</t>
+          <t>Normal</t>
         </is>
       </c>
       <c r="V15" t="inlineStr"/>
@@ -1978,103 +1986,600 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
+          <t>PED010</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>2025-10-23 12:30</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>2025-10-25 15:00</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>VIERNES</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Shopify</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>#SH1237</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>Valentina Rojas</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>+56956789012</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>Amor Eterno</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>Incluir tarjeta romántica</t>
+        </is>
+      </c>
+      <c r="K16" t="n">
+        <v>65000</v>
+      </c>
+      <c r="L16" t="n">
+        <v>7000</v>
+      </c>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>Sebastián Rojas</t>
+        </is>
+      </c>
+      <c r="N16" t="inlineStr">
+        <is>
+          <t>Eres el amor de mi vida</t>
+        </is>
+      </c>
+      <c r="O16" t="inlineStr">
+        <is>
+          <t>Valentina</t>
+        </is>
+      </c>
+      <c r="P16" t="inlineStr">
+        <is>
+          <t>Av. Las Condes 2345, Las Condes</t>
+        </is>
+      </c>
+      <c r="Q16" t="inlineStr">
+        <is>
+          <t>Las Condes</t>
+        </is>
+      </c>
+      <c r="R16" t="inlineStr">
+        <is>
+          <t>San Valentín</t>
+        </is>
+      </c>
+      <c r="S16" t="inlineStr">
+        <is>
+          <t>Entregas para Mañana</t>
+        </is>
+      </c>
+      <c r="T16" t="inlineStr">
+        <is>
+          <t>Pagado</t>
+        </is>
+      </c>
+      <c r="U16" t="inlineStr">
+        <is>
+          <t>EVENTO</t>
+        </is>
+      </c>
+      <c r="V16" t="inlineStr">
+        <is>
+          <t>FACTURA 2346 TR. 25/10/25</t>
+        </is>
+      </c>
+      <c r="W16" t="inlineStr"/>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>PED011</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>2025-10-23 16:20</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>2025-10-24 19:00</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>JUEVES</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>WhatsApp</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr"/>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>Diego Fernández</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>+56921098765</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>24 rosas rojas en ramo</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>URGENTE - Propuesta matrimonio</t>
+        </is>
+      </c>
+      <c r="K17" t="n">
+        <v>55000</v>
+      </c>
+      <c r="L17" t="n">
+        <v>10000</v>
+      </c>
+      <c r="M17" t="inlineStr">
+        <is>
+          <t>Camila Torres</t>
+        </is>
+      </c>
+      <c r="N17" t="inlineStr">
+        <is>
+          <t>¿Quieres casarte conmigo?</t>
+        </is>
+      </c>
+      <c r="O17" t="inlineStr">
+        <is>
+          <t>Diego</t>
+        </is>
+      </c>
+      <c r="P17" t="inlineStr">
+        <is>
+          <t>Av. Providencia 8901, Providencia</t>
+        </is>
+      </c>
+      <c r="Q17" t="inlineStr">
+        <is>
+          <t>Providencia</t>
+        </is>
+      </c>
+      <c r="R17" t="inlineStr">
+        <is>
+          <t>Propuesta</t>
+        </is>
+      </c>
+      <c r="S17" t="inlineStr">
+        <is>
+          <t>Pedidos Semana</t>
+        </is>
+      </c>
+      <c r="T17" t="inlineStr">
+        <is>
+          <t>Falta Boleta o Factura</t>
+        </is>
+      </c>
+      <c r="U17" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="V17" t="inlineStr"/>
+      <c r="W17" t="inlineStr"/>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>PED012</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>2025-10-23 15:45</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>2025-10-24 13:00</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>JUEVES</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Shopify</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>#SH1238</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>Carolina López</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>+56934567890</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>Elegancia Rosa</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr"/>
+      <c r="K18" t="n">
+        <v>38000</v>
+      </c>
+      <c r="L18" t="n">
+        <v>15000</v>
+      </c>
+      <c r="M18" t="inlineStr">
+        <is>
+          <t>Isabel López</t>
+        </is>
+      </c>
+      <c r="N18" t="inlineStr">
+        <is>
+          <t>Gracias por todo</t>
+        </is>
+      </c>
+      <c r="O18" t="inlineStr">
+        <is>
+          <t>Carolina</t>
+        </is>
+      </c>
+      <c r="P18" t="inlineStr">
+        <is>
+          <t>Av. Kennedy 3456, Vitacura</t>
+        </is>
+      </c>
+      <c r="Q18" t="inlineStr">
+        <is>
+          <t>Vitacura</t>
+        </is>
+      </c>
+      <c r="R18" t="inlineStr">
+        <is>
+          <t>Agradecimiento</t>
+        </is>
+      </c>
+      <c r="S18" t="inlineStr">
+        <is>
+          <t>Entregas de Hoy</t>
+        </is>
+      </c>
+      <c r="T18" t="inlineStr">
+        <is>
+          <t>No Pagado</t>
+        </is>
+      </c>
+      <c r="U18" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="V18" t="inlineStr"/>
+      <c r="W18" t="inlineStr"/>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>PED013</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>2025-10-23 17:00</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>2025-10-26 12:00</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>SABADO</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Shopify</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>#SH1239</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>Roberto Díaz</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>+56909876543</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>Arreglo Corporativo Mensual</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>Recepción empresa</t>
+        </is>
+      </c>
+      <c r="K19" t="n">
+        <v>80000</v>
+      </c>
+      <c r="L19" t="n">
+        <v>7000</v>
+      </c>
+      <c r="M19" t="inlineStr"/>
+      <c r="N19" t="inlineStr"/>
+      <c r="O19" t="inlineStr"/>
+      <c r="P19" t="inlineStr">
+        <is>
+          <t>Av. El Bosque 7890, Las Condes</t>
+        </is>
+      </c>
+      <c r="Q19" t="inlineStr">
+        <is>
+          <t>Las Condes</t>
+        </is>
+      </c>
+      <c r="R19" t="inlineStr">
+        <is>
+          <t>Corporativo</t>
+        </is>
+      </c>
+      <c r="S19" t="inlineStr">
+        <is>
+          <t>Pedidos Semana</t>
+        </is>
+      </c>
+      <c r="T19" t="inlineStr">
+        <is>
+          <t>Pagado</t>
+        </is>
+      </c>
+      <c r="U19" t="inlineStr">
+        <is>
+          <t>MANTENCIONES</t>
+        </is>
+      </c>
+      <c r="V19" t="inlineStr"/>
+      <c r="W19" t="inlineStr"/>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>PED014</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>2025-10-01 10:00</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>2025-10-02 09:00</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>MARTES</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Shopify</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>#SH1150</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>Roberto Díaz</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>+56909876543</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>Centro de Mesa Ejecutivo</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>Sala de reuniones</t>
+        </is>
+      </c>
+      <c r="K20" t="n">
+        <v>75000</v>
+      </c>
+      <c r="L20" t="n">
+        <v>7000</v>
+      </c>
+      <c r="M20" t="inlineStr"/>
+      <c r="N20" t="inlineStr"/>
+      <c r="O20" t="inlineStr"/>
+      <c r="P20" t="inlineStr">
+        <is>
+          <t>Av. El Bosque 7890, Las Condes</t>
+        </is>
+      </c>
+      <c r="Q20" t="inlineStr">
+        <is>
+          <t>Las Condes</t>
+        </is>
+      </c>
+      <c r="R20" t="inlineStr">
+        <is>
+          <t>Corporativo</t>
+        </is>
+      </c>
+      <c r="S20" t="inlineStr">
+        <is>
+          <t>Archivado</t>
+        </is>
+      </c>
+      <c r="T20" t="inlineStr">
+        <is>
+          <t>Pagado</t>
+        </is>
+      </c>
+      <c r="U20" t="inlineStr">
+        <is>
+          <t>MANTENCIONES</t>
+        </is>
+      </c>
+      <c r="V20" t="inlineStr"/>
+      <c r="W20" t="inlineStr"/>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
           <t>PED015</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr">
+      <c r="B21" t="inlineStr">
         <is>
           <t>2025-10-24 09:00</t>
         </is>
       </c>
-      <c r="C16" t="inlineStr">
+      <c r="C21" t="inlineStr">
         <is>
           <t>2025-10-25 14:00</t>
         </is>
       </c>
-      <c r="D16" t="inlineStr">
+      <c r="D21" t="inlineStr">
         <is>
           <t>VIERNES</t>
         </is>
       </c>
-      <c r="E16" t="inlineStr">
+      <c r="E21" t="inlineStr">
         <is>
           <t>WhatsApp</t>
         </is>
       </c>
-      <c r="F16" t="inlineStr"/>
-      <c r="G16" t="inlineStr">
+      <c r="F21" t="inlineStr"/>
+      <c r="G21" t="inlineStr">
         <is>
           <t>Pedro Silva</t>
         </is>
       </c>
-      <c r="H16" t="inlineStr">
+      <c r="H21" t="inlineStr">
         <is>
           <t>+56998765432</t>
         </is>
       </c>
-      <c r="I16" t="inlineStr">
+      <c r="I21" t="inlineStr">
         <is>
           <t>Ramo de Bienvenida</t>
         </is>
       </c>
-      <c r="J16" t="inlineStr">
+      <c r="J21" t="inlineStr">
         <is>
           <t>Primer pedido</t>
         </is>
       </c>
-      <c r="K16" t="n">
+      <c r="K21" t="n">
         <v>35000</v>
       </c>
-      <c r="L16" t="n">
+      <c r="L21" t="n">
         <v>15000</v>
       </c>
-      <c r="M16" t="inlineStr">
+      <c r="M21" t="inlineStr">
         <is>
           <t>Ana Silva</t>
         </is>
       </c>
-      <c r="N16" t="inlineStr">
+      <c r="N21" t="inlineStr">
         <is>
           <t>Bienvenida</t>
         </is>
       </c>
-      <c r="O16" t="inlineStr">
+      <c r="O21" t="inlineStr">
         <is>
           <t>Pedro</t>
         </is>
       </c>
-      <c r="P16" t="inlineStr">
+      <c r="P21" t="inlineStr">
         <is>
           <t>Av. Las Rejas 456, Estación Central</t>
         </is>
       </c>
-      <c r="Q16" t="inlineStr">
+      <c r="Q21" t="inlineStr">
         <is>
           <t>Estación Central</t>
         </is>
       </c>
-      <c r="R16" t="inlineStr">
+      <c r="R21" t="inlineStr">
         <is>
           <t>Otro</t>
         </is>
       </c>
-      <c r="S16" t="inlineStr">
+      <c r="S21" t="inlineStr">
         <is>
           <t>Pedido</t>
         </is>
       </c>
-      <c r="T16" t="inlineStr">
+      <c r="T21" t="inlineStr">
         <is>
           <t>No Pagado</t>
         </is>
       </c>
-      <c r="U16" t="inlineStr">
+      <c r="U21" t="inlineStr">
         <is>
           <t>Normal</t>
         </is>
       </c>
-      <c r="V16" t="inlineStr"/>
-      <c r="W16" t="inlineStr"/>
+      <c r="V21" t="inlineStr"/>
+      <c r="W21" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>